<commit_message>
modify data management web FE
</commit_message>
<xml_diff>
--- a/python-side/data/raw_data/genres.xlsx
+++ b/python-side/data/raw_data/genres.xlsx
@@ -426,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B20"/>
+  <dimension ref="A1:B18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -452,7 +452,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Fantasy</t>
+          <t>Romance</t>
         </is>
       </c>
     </row>
@@ -462,7 +462,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Documentary</t>
+          <t>Action</t>
         </is>
       </c>
     </row>
@@ -472,7 +472,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>War</t>
+          <t>Drama</t>
         </is>
       </c>
     </row>
@@ -482,7 +482,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Horror</t>
+          <t>Children</t>
         </is>
       </c>
     </row>
@@ -492,7 +492,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Children</t>
+          <t>Adventure</t>
         </is>
       </c>
     </row>
@@ -502,7 +502,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Mystery</t>
+          <t>Animation</t>
         </is>
       </c>
     </row>
@@ -512,7 +512,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Thriller</t>
+          <t>IMAX</t>
         </is>
       </c>
     </row>
@@ -522,7 +522,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Action</t>
+          <t>War</t>
         </is>
       </c>
     </row>
@@ -532,7 +532,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Comedy</t>
+          <t>Thriller</t>
         </is>
       </c>
     </row>
@@ -542,7 +542,7 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Drama</t>
+          <t>Comedy</t>
         </is>
       </c>
     </row>
@@ -562,7 +562,7 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>IMAX</t>
+          <t>Crime</t>
         </is>
       </c>
     </row>
@@ -572,7 +572,7 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Western</t>
+          <t>Fantasy</t>
         </is>
       </c>
     </row>
@@ -582,7 +582,7 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Adventure</t>
+          <t>Horror</t>
         </is>
       </c>
     </row>
@@ -592,7 +592,7 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Crime</t>
+          <t>Documentary</t>
         </is>
       </c>
     </row>
@@ -602,7 +602,7 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Film-Noir</t>
+          <t>Mystery</t>
         </is>
       </c>
     </row>
@@ -613,26 +613,6 @@
       <c r="B18" t="inlineStr">
         <is>
           <t>Sci-Fi</t>
-        </is>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="n">
-        <v>18</v>
-      </c>
-      <c r="B19" t="inlineStr">
-        <is>
-          <t>Romance</t>
-        </is>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="n">
-        <v>19</v>
-      </c>
-      <c r="B20" t="inlineStr">
-        <is>
-          <t>Animation</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
pagination +card mode + load by genre
</commit_message>
<xml_diff>
--- a/python-side/data/raw_data/genres.xlsx
+++ b/python-side/data/raw_data/genres.xlsx
@@ -457,7 +457,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Crime</t>
+          <t>Musical</t>
         </is>
       </c>
       <c r="C2" t="inlineStr"/>
@@ -468,7 +468,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Action</t>
+          <t>Film-Noir</t>
         </is>
       </c>
       <c r="C3" t="inlineStr"/>
@@ -479,7 +479,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Fantasy</t>
+          <t>Thriller</t>
         </is>
       </c>
       <c r="C4" t="inlineStr"/>
@@ -490,7 +490,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Comedy</t>
+          <t>Horror</t>
         </is>
       </c>
       <c r="C5" t="inlineStr"/>
@@ -501,7 +501,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>War</t>
+          <t>Action</t>
         </is>
       </c>
       <c r="C6" t="inlineStr"/>
@@ -512,7 +512,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Drama</t>
+          <t>Sci-Fi</t>
         </is>
       </c>
       <c r="C7" t="inlineStr"/>
@@ -534,7 +534,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Horror</t>
+          <t>Documentary</t>
         </is>
       </c>
       <c r="C9" t="inlineStr"/>
@@ -545,7 +545,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Sci-Fi</t>
+          <t>Crime</t>
         </is>
       </c>
       <c r="C10" t="inlineStr"/>
@@ -556,7 +556,7 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>IMAX</t>
+          <t>Drama</t>
         </is>
       </c>
       <c r="C11" t="inlineStr"/>
@@ -567,7 +567,7 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Film-Noir</t>
+          <t>Western</t>
         </is>
       </c>
       <c r="C12" t="inlineStr"/>
@@ -578,7 +578,7 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Documentary</t>
+          <t>Adventure</t>
         </is>
       </c>
       <c r="C13" t="inlineStr"/>
@@ -589,7 +589,7 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Romance</t>
+          <t>War</t>
         </is>
       </c>
       <c r="C14" t="inlineStr"/>
@@ -611,7 +611,7 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Mystery</t>
+          <t>Romance</t>
         </is>
       </c>
       <c r="C16" t="inlineStr"/>
@@ -622,7 +622,7 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Western</t>
+          <t>Mystery</t>
         </is>
       </c>
       <c r="C17" t="inlineStr"/>
@@ -633,7 +633,7 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Thriller</t>
+          <t>Comedy</t>
         </is>
       </c>
       <c r="C18" t="inlineStr"/>
@@ -644,7 +644,7 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Adventure</t>
+          <t>IMAX</t>
         </is>
       </c>
       <c r="C19" t="inlineStr"/>
@@ -655,7 +655,7 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Musical</t>
+          <t>Fantasy</t>
         </is>
       </c>
       <c r="C20" t="inlineStr"/>

</xml_diff>